<commit_message>
Modifed CR calculation and Correct the test data
</commit_message>
<xml_diff>
--- a/td_toolkits_v3/opticals/tests/test_files/properties/batch_upload_test.xlsx
+++ b/td_toolkits_v3/opticals/tests/test_files/properties/batch_upload_test.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1875" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LiquidCrystal" sheetId="1" r:id="rId1"/>
     <sheet name="Polyimide" sheetId="2" r:id="rId2"/>
     <sheet name="Seal" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +150,12 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -171,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -179,6 +185,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -461,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -470,11 +477,12 @@
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="1" customWidth="1"/>
-    <col min="9" max="11" width="5.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="3.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="14.5703125" style="1" customWidth="1"/>
     <col min="12" max="14" width="11" style="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="1" customWidth="1"/>
     <col min="16" max="1024" width="9.140625" style="1"/>
@@ -527,7 +535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -543,29 +551,29 @@
       <c r="G2" s="1">
         <v>83</v>
       </c>
-      <c r="H2" s="1">
-        <v>1.58</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1.48</v>
+      <c r="H2" s="5">
+        <v>1.5769</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1.4806999999999999</v>
       </c>
       <c r="J2" s="1">
-        <v>1.58</v>
+        <v>3.5</v>
       </c>
       <c r="K2" s="1">
-        <v>1.48</v>
-      </c>
-      <c r="L2" s="1">
-        <v>14.7</v>
-      </c>
-      <c r="M2" s="1">
-        <v>7.35</v>
-      </c>
-      <c r="N2" s="1">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.8</v>
+      </c>
+      <c r="L2" s="5">
+        <v>14</v>
+      </c>
+      <c r="M2" s="5">
+        <v>7</v>
+      </c>
+      <c r="N2" s="5">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -581,17 +589,17 @@
       <c r="G3" s="1">
         <v>97</v>
       </c>
-      <c r="H3" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1.49</v>
+      <c r="H3" s="5">
+        <v>1.6028</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1.4877</v>
       </c>
       <c r="J3" s="1">
-        <v>1.6</v>
+        <v>3.85</v>
       </c>
       <c r="K3" s="1">
-        <v>1.49</v>
+        <v>8.08</v>
       </c>
       <c r="L3" s="1">
         <v>17</v>
@@ -603,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -619,17 +627,17 @@
       <c r="G4" s="1">
         <v>76</v>
       </c>
-      <c r="H4" s="1">
-        <v>1.59</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1.48</v>
+      <c r="H4" s="5">
+        <v>1.5868</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.4842</v>
       </c>
       <c r="J4" s="1">
-        <v>1.59</v>
+        <v>3.61</v>
       </c>
       <c r="K4" s="1">
-        <v>1.48</v>
+        <v>6.39</v>
       </c>
       <c r="L4" s="1">
         <v>14.6</v>
@@ -641,7 +649,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -657,17 +665,17 @@
       <c r="G5" s="1">
         <v>53</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="5">
         <v>1.59</v>
       </c>
-      <c r="I5" s="1">
-        <v>1.49</v>
+      <c r="I5" s="5">
+        <v>1.486</v>
       </c>
       <c r="J5" s="1">
-        <v>1.59</v>
+        <v>3.46</v>
       </c>
       <c r="K5" s="1">
-        <v>1.49</v>
+        <v>6.9</v>
       </c>
       <c r="L5" s="1">
         <v>15.4</v>
@@ -679,7 +687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -695,17 +703,17 @@
       <c r="G6" s="1">
         <v>88</v>
       </c>
-      <c r="H6" s="1">
-        <v>1.59</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1.49</v>
+      <c r="H6" s="5">
+        <v>1.5891</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.4857</v>
       </c>
       <c r="J6" s="1">
-        <v>1.59</v>
+        <v>3.45</v>
       </c>
       <c r="K6" s="1">
-        <v>1.49</v>
+        <v>6.6</v>
       </c>
       <c r="L6" s="1">
         <v>13.5</v>
@@ -761,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>